<commit_message>
Excel read Print value
</commit_message>
<xml_diff>
--- a/EmployeeManagement/TestData/orange_data.xlsx
+++ b/EmployeeManagement/TestData/orange_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patilbs\Desktop\C#\Automationframework\EmployeeManagement\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EB25D5-424C-4F01-ADB2-C966C0496044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C144DD5-0D35-46EF-A1FA-9F952D5EE1C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Username</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>John123</t>
+  </si>
+  <si>
+    <t>peter</t>
+  </si>
+  <si>
+    <t>peter123</t>
   </si>
 </sst>
 </file>
@@ -369,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -414,6 +420,17 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Read data from Excel
</commit_message>
<xml_diff>
--- a/EmployeeManagement/TestData/orange_data.xlsx
+++ b/EmployeeManagement/TestData/orange_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patilbs\Desktop\C#\Automationframework\EmployeeManagement\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C144DD5-0D35-46EF-A1FA-9F952D5EE1C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B95263-5153-4B92-BCE4-2CF6915EF10B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Username</t>
   </si>
@@ -52,12 +52,6 @@
   </si>
   <si>
     <t>John123</t>
-  </si>
-  <si>
-    <t>peter</t>
-  </si>
-  <si>
-    <t>peter123</t>
   </si>
 </sst>
 </file>
@@ -375,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -420,17 +414,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>